<commit_message>
full implementation of the solver with hard constraints. soft constraints remain to be implemented.
</commit_message>
<xml_diff>
--- a/timetable-generator/Tables.xlsx
+++ b/timetable-generator/Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\OneDrive - Egypt Japan University Of Science and Technology (E-JUST)\CSIT Assignments\Year 3\Semester 1\Intillegent Systems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\ubuntu\home\eyad\timetable-generator\timetable-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54ADE195-CB2C-44AC-AB6B-434DDF7CB616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921367F7-3630-4A86-B401-C7EAD17820E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19095" windowHeight="12075" xr2:uid="{150013C0-0388-42A9-86A1-272095128D9A}"/>
+    <workbookView xWindow="15" yWindow="375" windowWidth="18885" windowHeight="11865" activeTab="1" xr2:uid="{150013C0-0388-42A9-86A1-272095128D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="226">
   <si>
     <t>course_id</t>
   </si>
@@ -128,9 +128,6 @@
     <t>ACM 215</t>
   </si>
   <si>
-    <t xml:space="preserve"> LRA 403</t>
-  </si>
-  <si>
     <t>Japanese Language (3)</t>
   </si>
   <si>
@@ -711,6 +708,18 @@
   </si>
   <si>
     <t xml:space="preserve">AID 321 </t>
+  </si>
+  <si>
+    <t>group_number</t>
+  </si>
+  <si>
+    <t>Bottleneck</t>
+  </si>
+  <si>
+    <t>AID 427, AID 428</t>
+  </si>
+  <si>
+    <t>CNC 111, AID 427</t>
   </si>
 </sst>
 </file>
@@ -773,7 +782,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -803,13 +831,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6792FEB4-48DE-45AC-BEAE-E1754499E8F6}" name="Table3" displayName="Table3" ref="A1:D47" totalsRowShown="0">
-  <autoFilter ref="A1:D47" xr:uid="{6792FEB4-48DE-45AC-BEAE-E1754499E8F6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D44">
-    <sortCondition ref="B1:B44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6792FEB4-48DE-45AC-BEAE-E1754499E8F6}" name="Table3" displayName="Table3" ref="A1:D48" totalsRowShown="0">
+  <autoFilter ref="A1:D48" xr:uid="{6792FEB4-48DE-45AC-BEAE-E1754499E8F6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D48">
+    <sortCondition ref="D1:D48"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{15396D68-3FEE-46AF-873C-518F133DA045}" name="instructor_id" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{15396D68-3FEE-46AF-873C-518F133DA045}" name="instructor_id" dataDxfId="1">
       <calculatedColumnFormula>ROW() - ROW(Table3[[#Headers],[instructor_id]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{47DB9175-F9E8-4552-A4C5-6D044C11CC2A}" name="name"/>
@@ -849,10 +877,11 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4FBF574A-2262-47D1-9435-34D26646F02E}" name="Table5" displayName="Table5" ref="A1:C37" totalsRowShown="0">
-  <autoFilter ref="A1:C37" xr:uid="{4FBF574A-2262-47D1-9435-34D26646F02E}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4FBF574A-2262-47D1-9435-34D26646F02E}" name="Table5" displayName="Table5" ref="A1:D37" totalsRowShown="0">
+  <autoFilter ref="A1:D37" xr:uid="{4FBF574A-2262-47D1-9435-34D26646F02E}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8D629C59-2D54-4EAD-AB23-9FA6480DF5A4}" name="section_id"/>
+    <tableColumn id="4" xr3:uid="{B94BD765-4F5A-4343-95C4-C724CF2925EB}" name="group_number" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{1F3C2032-D4C6-4EF1-B961-24FCDB625962}" name="year"/>
     <tableColumn id="3" xr3:uid="{9A64CE56-6DDA-41DA-8CF0-218A5801A281}" name="student_count"/>
   </tableColumns>
@@ -1173,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAC10A2-0620-4AD0-AC86-CF3FB68295CE}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1307,10 +1336,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1318,10 +1347,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1329,10 +1358,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1340,10 +1369,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -1351,10 +1380,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -1362,10 +1391,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -1373,10 +1402,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1384,10 +1413,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -1395,10 +1424,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
@@ -1406,10 +1435,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1417,10 +1446,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1428,10 +1457,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
@@ -1439,10 +1468,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
@@ -1450,10 +1479,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -1461,10 +1490,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
@@ -1472,21 +1501,21 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
         <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
         <v>16</v>
@@ -1494,10 +1523,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
         <v>16</v>
@@ -1505,10 +1534,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -1524,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB8F337-374A-4E48-B90C-47DDE19CF40A}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1540,16 +1569,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -1558,13 +1587,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -1573,13 +1602,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -1588,13 +1617,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -1603,13 +1632,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -1618,13 +1647,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -1633,13 +1662,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>223</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -1648,13 +1677,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -1663,13 +1692,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -1678,13 +1707,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -1693,13 +1722,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -1708,13 +1737,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
@@ -1723,13 +1752,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -1738,13 +1767,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
@@ -1753,13 +1782,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
@@ -1768,13 +1797,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -1783,13 +1812,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -1797,14 +1826,14 @@
         <f>ROW() - ROW(Table3[[#Headers],[instructor_id]])</f>
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>100</v>
+      <c r="B18" t="s">
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
@@ -1813,13 +1842,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -1828,13 +1857,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -1843,13 +1872,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
@@ -1858,13 +1887,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
@@ -1873,13 +1902,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
@@ -1888,13 +1917,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
@@ -1903,13 +1932,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
@@ -1918,13 +1947,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
@@ -1932,14 +1961,14 @@
         <f>ROW() - ROW(Table3[[#Headers],[instructor_id]])</f>
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>126</v>
+      <c r="B27" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
@@ -1948,13 +1977,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
@@ -1963,13 +1992,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
         <v>76</v>
       </c>
-      <c r="C29" t="s">
-        <v>77</v>
-      </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
@@ -1978,13 +2007,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>118</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
@@ -1993,13 +2022,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>130</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
@@ -2008,13 +2037,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
@@ -2023,13 +2052,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
@@ -2038,13 +2067,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
@@ -2053,13 +2082,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D35" t="s">
-        <v>138</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
@@ -2068,13 +2097,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
@@ -2083,13 +2112,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>219</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
@@ -2098,13 +2127,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
@@ -2113,13 +2142,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D39" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
@@ -2128,13 +2157,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D40" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
@@ -2143,13 +2172,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
@@ -2158,13 +2187,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
@@ -2173,13 +2202,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
@@ -2188,13 +2217,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D44" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
@@ -2203,13 +2232,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
@@ -2218,13 +2247,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="D46" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
@@ -2233,13 +2262,28 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>220</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D47" t="s">
-        <v>219</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" s="2">
+        <f>ROW() - ROW(Table3[[#Headers],[instructor_id]])</f>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2254,8 +2298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D74D33-1FE0-4647-A041-3A11F9673EDB}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2267,18 +2311,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -2289,7 +2333,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -2300,10 +2344,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -2311,7 +2355,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -2322,7 +2366,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -2333,7 +2377,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -2344,7 +2388,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -2355,7 +2399,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -2366,7 +2410,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -2377,10 +2421,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11">
         <v>15</v>
@@ -2388,10 +2432,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C12">
         <v>45</v>
@@ -2399,10 +2443,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13">
         <v>30</v>
@@ -2410,10 +2454,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C14">
         <v>15</v>
@@ -2421,10 +2465,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15">
         <v>15</v>
@@ -2432,10 +2476,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16">
         <v>30</v>
@@ -2443,7 +2487,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -2454,7 +2498,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -2465,7 +2509,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -2476,7 +2520,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -2487,7 +2531,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
@@ -2498,7 +2542,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -2509,7 +2553,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
@@ -2520,7 +2564,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
@@ -2531,7 +2575,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -2542,7 +2586,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
@@ -2553,7 +2597,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -2564,7 +2608,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -2575,7 +2619,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -2586,7 +2630,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
@@ -2597,7 +2641,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
@@ -2608,7 +2652,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -2619,10 +2663,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C33">
         <v>15</v>
@@ -2630,10 +2674,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C34">
         <v>15</v>
@@ -2641,10 +2685,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C35">
         <v>15</v>
@@ -2652,10 +2696,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C36">
         <v>15</v>
@@ -2663,7 +2707,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
@@ -2674,10 +2718,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" t="s">
         <v>148</v>
-      </c>
-      <c r="B38" t="s">
-        <v>149</v>
       </c>
       <c r="C38">
         <v>45</v>
@@ -2685,10 +2729,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C39">
         <v>45</v>
@@ -2696,7 +2740,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -2707,7 +2751,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -2718,7 +2762,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -2729,7 +2773,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -2740,7 +2784,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -2775,24 +2819,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" t="s">
         <v>186</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>187</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>188</v>
-      </c>
-      <c r="D1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="C2" s="4">
         <v>0.375</v>
@@ -2803,10 +2847,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" s="4">
         <v>0.44791666666666669</v>
@@ -2817,10 +2861,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" s="4">
         <v>0.52083333333333337</v>
@@ -2831,10 +2875,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C5" s="4">
         <v>9.375E-2</v>
@@ -2845,10 +2889,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="C6" s="4">
         <v>0.375</v>
@@ -2859,10 +2903,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" s="4">
         <v>0.44791666666666669</v>
@@ -2873,10 +2917,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C8" s="4">
         <v>0.52083333333333337</v>
@@ -2887,10 +2931,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C9" s="4">
         <v>9.375E-2</v>
@@ -2901,10 +2945,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="C10" s="4">
         <v>0.375</v>
@@ -2915,10 +2959,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" s="4">
         <v>0.44791666666666669</v>
@@ -2929,10 +2973,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" s="4">
         <v>0.52083333333333337</v>
@@ -2943,10 +2987,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C13" s="4">
         <v>9.375E-2</v>
@@ -2957,10 +3001,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="C14" s="4">
         <v>0.375</v>
@@ -2971,10 +3015,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C15" s="4">
         <v>0.44791666666666669</v>
@@ -2985,10 +3029,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C16" s="4">
         <v>0.52083333333333337</v>
@@ -2999,10 +3043,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C17" s="4">
         <v>9.375E-2</v>
@@ -3013,10 +3057,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="C18" s="4">
         <v>0.375</v>
@@ -3027,10 +3071,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C19" s="4">
         <v>0.44791666666666669</v>
@@ -3041,10 +3085,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C20" s="4">
         <v>0.52083333333333337</v>
@@ -3055,10 +3099,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C21" s="4">
         <v>9.375E-2</v>
@@ -3078,31 +3122,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8B76FE-50C2-469C-98CB-EE21A2F0AF79}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection sqref="A1:C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.796875" customWidth="1"/>
-    <col min="2" max="2" width="13.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.06640625" customWidth="1"/>
     <col min="3" max="3" width="14.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" t="s">
         <v>215</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>216</v>
       </c>
-      <c r="C1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3110,10 +3157,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3121,10 +3171,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3132,109 +3185,139 @@
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="C7" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="5">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5">
         <v>1</v>
       </c>
-      <c r="C8" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="5">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="5">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5">
         <v>1</v>
       </c>
-      <c r="C10" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>1</v>
       </c>
       <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
         <v>2</v>
       </c>
-      <c r="C11" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D11" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>2</v>
       </c>
       <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>3</v>
       </c>
       <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
         <v>2</v>
       </c>
-      <c r="C13" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D13" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>4</v>
       </c>
@@ -3242,10 +3325,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>5</v>
       </c>
@@ -3253,10 +3339,13 @@
         <v>2</v>
       </c>
       <c r="C15" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>6</v>
       </c>
@@ -3264,109 +3353,139 @@
         <v>2</v>
       </c>
       <c r="C16" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>7</v>
       </c>
       <c r="B17" s="5">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5">
         <v>2</v>
       </c>
-      <c r="C17" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>8</v>
       </c>
       <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5">
         <v>2</v>
       </c>
-      <c r="C18" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>9</v>
       </c>
       <c r="B19" s="5">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5">
         <v>2</v>
       </c>
-      <c r="C19" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>1</v>
       </c>
       <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5">
         <v>3</v>
       </c>
-      <c r="C20" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>2</v>
       </c>
       <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
         <v>3</v>
       </c>
-      <c r="C21" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>3</v>
       </c>
       <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
         <v>3</v>
       </c>
-      <c r="C22" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D22" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>4</v>
       </c>
       <c r="B23" s="5">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5">
         <v>3</v>
       </c>
-      <c r="C23" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D23" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>5</v>
       </c>
       <c r="B24" s="5">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5">
         <v>3</v>
       </c>
-      <c r="C24" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D24" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>6</v>
       </c>
       <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" s="5">
         <v>3</v>
       </c>
-      <c r="C25" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D25" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
         <v>7</v>
       </c>
@@ -3374,10 +3493,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
         <v>8</v>
       </c>
@@ -3385,10 +3507,13 @@
         <v>3</v>
       </c>
       <c r="C27" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="D27" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>9</v>
       </c>
@@ -3396,105 +3521,135 @@
         <v>3</v>
       </c>
       <c r="C28" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
         <v>1</v>
       </c>
       <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
         <v>4</v>
       </c>
-      <c r="C29" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D29" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
         <v>2</v>
       </c>
       <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
         <v>4</v>
       </c>
-      <c r="C30" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D30" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>3</v>
       </c>
       <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5">
         <v>4</v>
       </c>
-      <c r="C31" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
         <v>4</v>
       </c>
       <c r="B32" s="5">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5">
         <v>4</v>
       </c>
-      <c r="C32" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="5">
         <v>5</v>
       </c>
       <c r="B33" s="5">
+        <v>2</v>
+      </c>
+      <c r="C33" s="5">
         <v>4</v>
       </c>
-      <c r="C33" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D33" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="5">
         <v>6</v>
       </c>
       <c r="B34" s="5">
+        <v>2</v>
+      </c>
+      <c r="C34" s="5">
         <v>4</v>
       </c>
-      <c r="C34" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D34" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
         <v>7</v>
       </c>
       <c r="B35" s="5">
+        <v>3</v>
+      </c>
+      <c r="C35" s="5">
         <v>4</v>
       </c>
-      <c r="C35" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D35" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="5">
         <v>8</v>
       </c>
       <c r="B36" s="5">
+        <v>3</v>
+      </c>
+      <c r="C36" s="5">
         <v>4</v>
       </c>
-      <c r="C36" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D36" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="5">
         <v>9</v>
       </c>
       <c r="B37" s="5">
+        <v>3</v>
+      </c>
+      <c r="C37" s="5">
         <v>4</v>
       </c>
-      <c r="C37" s="5">
+      <c r="D37" s="5">
         <v>15</v>
       </c>
     </row>
@@ -3523,7 +3678,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3566,7 +3721,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -3606,7 +3761,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -3614,7 +3769,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -3630,7 +3785,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -3638,7 +3793,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -3646,7 +3801,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -3662,7 +3817,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
@@ -3670,7 +3825,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
@@ -3678,7 +3833,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -3686,7 +3841,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
@@ -3694,7 +3849,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
@@ -3702,7 +3857,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
@@ -3710,7 +3865,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
@@ -3718,7 +3873,7 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
@@ -3726,7 +3881,7 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
@@ -3734,7 +3889,7 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
@@ -3742,7 +3897,7 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
@@ -3750,7 +3905,7 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
@@ -3758,7 +3913,7 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished up the solver with hard and soft constraints along with the two modes "FIND_FIRST" and "OPTIMIZE"
</commit_message>
<xml_diff>
--- a/timetable-generator/Tables.xlsx
+++ b/timetable-generator/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\ubuntu\home\eyad\timetable-generator\timetable-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921367F7-3630-4A86-B401-C7EAD17820E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2F187D-701D-40E9-835D-C476254BBAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="375" windowWidth="18885" windowHeight="11865" activeTab="1" xr2:uid="{150013C0-0388-42A9-86A1-272095128D9A}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="18885" windowHeight="11865" activeTab="3" xr2:uid="{150013C0-0388-42A9-86A1-272095128D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="2" r:id="rId1"/>
@@ -772,17 +772,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
       <font>
         <b val="0"/>
@@ -801,6 +801,12 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -837,7 +843,7 @@
     <sortCondition ref="D1:D48"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{15396D68-3FEE-46AF-873C-518F133DA045}" name="instructor_id" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{15396D68-3FEE-46AF-873C-518F133DA045}" name="instructor_id" dataDxfId="3">
       <calculatedColumnFormula>ROW() - ROW(Table3[[#Headers],[instructor_id]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{47DB9175-F9E8-4552-A4C5-6D044C11CC2A}" name="name"/>
@@ -869,8 +875,8 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{ED0EDD08-E72C-4741-914F-8630C3E146E5}" name="time_slot_id"/>
     <tableColumn id="2" xr3:uid="{3BF236E5-3EE0-4484-9DA6-96118DC1ED66}" name="day"/>
-    <tableColumn id="3" xr3:uid="{088B2E27-F249-4438-9A52-625B6326BF4F}" name="start_time"/>
-    <tableColumn id="4" xr3:uid="{4E0CC6BF-DC4B-43B6-971B-E8992A81E37C}" name="end_time"/>
+    <tableColumn id="3" xr3:uid="{088B2E27-F249-4438-9A52-625B6326BF4F}" name="start_time" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4E0CC6BF-DC4B-43B6-971B-E8992A81E37C}" name="end_time" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1555,7 +1561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB8F337-374A-4E48-B90C-47DDE19CF40A}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -2805,8 +2811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5170881-DCFD-4CBD-B8FA-DD9363B6F7C2}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2838,10 +2844,10 @@
       <c r="B2" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>0.375</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>0.4375</v>
       </c>
     </row>
@@ -2852,10 +2858,10 @@
       <c r="B3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>0.51041666666666663</v>
       </c>
     </row>
@@ -2866,11 +2872,11 @@
       <c r="B4" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>0.52083333333333337</v>
       </c>
-      <c r="D4" s="4">
-        <v>8.3333333333333329E-2</v>
+      <c r="D4" s="5">
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -2880,11 +2886,11 @@
       <c r="B5" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C5" s="4">
-        <v>9.375E-2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.15625</v>
+      <c r="C5" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.65625</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -2894,10 +2900,10 @@
       <c r="B6" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>0.375</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>0.4375</v>
       </c>
     </row>
@@ -2908,10 +2914,10 @@
       <c r="B7" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>0.51041666666666663</v>
       </c>
     </row>
@@ -2922,11 +2928,11 @@
       <c r="B8" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>0.52083333333333337</v>
       </c>
-      <c r="D8" s="4">
-        <v>8.3333333333333329E-2</v>
+      <c r="D8" s="5">
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -2936,11 +2942,11 @@
       <c r="B9" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C9" s="4">
-        <v>9.375E-2</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.15625</v>
+      <c r="C9" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.65625</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -2950,10 +2956,10 @@
       <c r="B10" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>0.375</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <v>0.4375</v>
       </c>
     </row>
@@ -2964,10 +2970,10 @@
       <c r="B11" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="5">
         <v>0.51041666666666663</v>
       </c>
     </row>
@@ -2978,11 +2984,11 @@
       <c r="B12" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>0.52083333333333337</v>
       </c>
-      <c r="D12" s="4">
-        <v>8.3333333333333329E-2</v>
+      <c r="D12" s="5">
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
@@ -2992,11 +2998,11 @@
       <c r="B13" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C13" s="4">
-        <v>9.375E-2</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.15625</v>
+      <c r="C13" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.65625</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -3006,10 +3012,10 @@
       <c r="B14" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <v>0.375</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="5">
         <v>0.4375</v>
       </c>
     </row>
@@ -3020,10 +3026,10 @@
       <c r="B15" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="5">
         <v>0.51041666666666663</v>
       </c>
     </row>
@@ -3034,11 +3040,11 @@
       <c r="B16" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>0.52083333333333337</v>
       </c>
-      <c r="D16" s="4">
-        <v>8.3333333333333329E-2</v>
+      <c r="D16" s="5">
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -3048,11 +3054,11 @@
       <c r="B17" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C17" s="4">
-        <v>9.375E-2</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.15625</v>
+      <c r="C17" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.65625</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -3062,10 +3068,10 @@
       <c r="B18" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <v>0.375</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="5">
         <v>0.4375</v>
       </c>
     </row>
@@ -3076,10 +3082,10 @@
       <c r="B19" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="5">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="5">
         <v>0.51041666666666663</v>
       </c>
     </row>
@@ -3090,11 +3096,11 @@
       <c r="B20" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="5">
         <v>0.52083333333333337</v>
       </c>
-      <c r="D20" s="4">
-        <v>8.3333333333333329E-2</v>
+      <c r="D20" s="5">
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -3104,11 +3110,11 @@
       <c r="B21" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C21" s="4">
-        <v>9.375E-2</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0.15625</v>
+      <c r="C21" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.65625</v>
       </c>
     </row>
   </sheetData>
@@ -3150,506 +3156,506 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>1</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>1</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>3</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>1</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>2</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>4</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>2</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>2</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>5</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>2</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>6</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>2</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>2</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>7</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>3</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>2</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>8</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>3</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>2</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>9</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>3</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>2</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>1</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>1</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>3</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>2</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>1</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>3</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>3</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>1</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>3</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>4</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>2</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>3</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>5</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>2</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>3</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>6</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>2</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>3</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>7</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>3</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>3</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>8</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>3</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>3</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>9</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>3</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>3</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="5">
+      <c r="A29" s="4">
         <v>1</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>1</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>4</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>2</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>1</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>4</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>3</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>1</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>4</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>4</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>2</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>4</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" s="5">
+      <c r="A33" s="4">
         <v>5</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="4">
         <v>2</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <v>4</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>6</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>2</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="4">
         <v>4</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="5">
+      <c r="A35" s="4">
         <v>7</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="4">
         <v>3</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="4">
         <v>4</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="5">
+      <c r="A36" s="4">
         <v>8</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>3</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="4">
         <v>4</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" s="5">
+      <c r="A37" s="4">
         <v>9</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>3</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="4">
         <v>4</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="4">
         <v>15</v>
       </c>
     </row>

</xml_diff>